<commit_message>
Adding Joshua Tree info
</commit_message>
<xml_diff>
--- a/events/Joshua_Tree_2019/JoshuaTree2019.xlsx
+++ b/events/Joshua_Tree_2019/JoshuaTree2019.xlsx
@@ -10,17 +10,14 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$48</definedName>
+    <definedName name="_xlnm.Print_Area" localSheetId="0">Sheet1!$A$1:$G$57</definedName>
   </definedNames>
   <calcPr calcId="152511"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="59" uniqueCount="48">
-  <si>
-    <t>Cost: $35</t>
-  </si>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
   <si>
     <t>Patrol</t>
   </si>
@@ -31,27 +28,15 @@
     <t>Permission Slip</t>
   </si>
   <si>
-    <t>Wolverine</t>
-  </si>
-  <si>
     <t>Tommy Herro</t>
   </si>
   <si>
-    <t>Zachary Hofsaess</t>
-  </si>
-  <si>
     <t>Evan Maclean</t>
   </si>
   <si>
-    <t>Dan Lavallee</t>
-  </si>
-  <si>
     <t>Dylan Schuster</t>
   </si>
   <si>
-    <t>car</t>
-  </si>
-  <si>
     <t>Adult</t>
   </si>
   <si>
@@ -85,9 +70,6 @@
     <t>Who</t>
   </si>
   <si>
-    <t>Raccoon</t>
-  </si>
-  <si>
     <t>12 pm pick up</t>
   </si>
   <si>
@@ -161,12 +143,78 @@
   </si>
   <si>
     <t>Recreation.gov</t>
+  </si>
+  <si>
+    <t>John Paul Pauly</t>
+  </si>
+  <si>
+    <t>Simon Pauly</t>
+  </si>
+  <si>
+    <t>Dion Cleghorn Roer</t>
+  </si>
+  <si>
+    <t>Justin Arita</t>
+  </si>
+  <si>
+    <t>Scout</t>
+  </si>
+  <si>
+    <t>Stephan</t>
+  </si>
+  <si>
+    <t>Schuster</t>
+  </si>
+  <si>
+    <t>chk</t>
+  </si>
+  <si>
+    <t>x</t>
+  </si>
+  <si>
+    <t>groceries</t>
+  </si>
+  <si>
+    <t>Cost:</t>
+  </si>
+  <si>
+    <t>checks to deposit</t>
+  </si>
+  <si>
+    <t>Stephan SA</t>
+  </si>
+  <si>
+    <t>Schuster SA</t>
+  </si>
+  <si>
+    <t>Maclean SA</t>
+  </si>
+  <si>
+    <t>Lavallee SA</t>
+  </si>
+  <si>
+    <t>Herro SA</t>
+  </si>
+  <si>
+    <t>Dion Roer SA</t>
+  </si>
+  <si>
+    <t>Arita SA</t>
+  </si>
+  <si>
+    <t>debit</t>
+  </si>
+  <si>
+    <t>credit to Schuster account</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <numFmts count="1">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -284,7 +332,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="19">
+  <cellXfs count="21">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -302,6 +350,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -615,10 +665,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G59"/>
+  <dimension ref="A1:G57"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="C40" sqref="C40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection sqref="A1:G57"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -634,32 +684,32 @@
   <sheetData>
     <row r="1" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>31</v>
+        <v>25</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>32</v>
+        <v>26</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>23</v>
+        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D2" t="s">
-        <v>24</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>25</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="13" t="s">
-        <v>44</v>
+        <v>38</v>
       </c>
       <c r="B3" s="14" t="s">
-        <v>45</v>
+        <v>39</v>
       </c>
       <c r="C3" s="14"/>
       <c r="D3" s="14"/>
@@ -686,15 +736,15 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="17" t="s">
-        <v>46</v>
-      </c>
-      <c r="B6" s="17"/>
-      <c r="C6" s="17"/>
-      <c r="D6" s="17"/>
-      <c r="E6" s="17"/>
-      <c r="F6" s="17"/>
-      <c r="G6" s="18"/>
+      <c r="A6" s="19" t="s">
+        <v>40</v>
+      </c>
+      <c r="B6" s="19"/>
+      <c r="C6" s="19"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
+      <c r="F6" s="19"/>
+      <c r="G6" s="20"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
@@ -716,25 +766,28 @@
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>0</v>
+        <v>52</v>
+      </c>
+      <c r="B10" s="1">
+        <v>35</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="12" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B12" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="3" t="s">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="s">
+      <c r="D12" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="D12" s="3" t="s">
-        <v>3</v>
-      </c>
       <c r="E12" s="3" t="s">
-        <v>16</v>
+        <v>11</v>
       </c>
       <c r="F12" s="3"/>
       <c r="G12" s="4"/>
@@ -750,16 +803,16 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="5" t="s">
-        <v>33</v>
+        <v>27</v>
       </c>
       <c r="B14" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="C14" s="6" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D14" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E14" s="6"/>
       <c r="F14" s="6"/>
@@ -767,16 +820,16 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B15" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C15" s="6" t="s">
         <v>7</v>
       </c>
-      <c r="B15" s="6" t="s">
-        <v>34</v>
-      </c>
-      <c r="C15" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="D15" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E15" s="6"/>
       <c r="F15" s="6"/>
@@ -784,14 +837,14 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5" t="s">
-        <v>35</v>
+        <v>29</v>
       </c>
       <c r="B16" s="6"/>
       <c r="C16" s="6" t="s">
-        <v>34</v>
+        <v>7</v>
       </c>
       <c r="D16" s="6" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E16" s="6"/>
       <c r="F16" s="6"/>
@@ -799,57 +852,87 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="5" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="B17" s="6"/>
-      <c r="C17" s="6"/>
-      <c r="D17" s="6"/>
+      <c r="C17" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D17" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
       <c r="G17" s="7"/>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="5" t="s">
-        <v>6</v>
+        <v>42</v>
       </c>
       <c r="B18" s="6"/>
-      <c r="C18" s="8"/>
-      <c r="D18" s="6"/>
+      <c r="C18" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D18" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
       <c r="G18" s="7"/>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A19" s="5"/>
+      <c r="A19" s="5" t="s">
+        <v>43</v>
+      </c>
       <c r="B19" s="6"/>
-      <c r="C19" s="8"/>
-      <c r="D19" s="6"/>
+      <c r="C19" s="8" t="s">
+        <v>49</v>
+      </c>
+      <c r="D19" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="E19" s="6"/>
       <c r="F19" s="8"/>
       <c r="G19" s="7"/>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A20" s="5"/>
+      <c r="A20" s="5" t="s">
+        <v>44</v>
+      </c>
       <c r="B20" s="6"/>
-      <c r="C20" s="6"/>
-      <c r="D20" s="8"/>
+      <c r="C20" s="8" t="s">
+        <v>7</v>
+      </c>
+      <c r="D20" s="8" t="s">
+        <v>50</v>
+      </c>
       <c r="E20" s="6"/>
       <c r="F20" s="8"/>
       <c r="G20" s="7"/>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A21" s="5"/>
+      <c r="A21" s="5" t="s">
+        <v>45</v>
+      </c>
       <c r="B21" s="6"/>
-      <c r="C21" s="6"/>
+      <c r="C21" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
       <c r="F21" s="8"/>
       <c r="G21" s="7"/>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A22" s="5"/>
-      <c r="B22" s="6"/>
-      <c r="C22" s="6"/>
+      <c r="A22" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="B22" s="6" t="s">
+        <v>34</v>
+      </c>
+      <c r="C22" s="8" t="s">
+        <v>7</v>
+      </c>
       <c r="D22" s="8"/>
       <c r="E22" s="6"/>
       <c r="F22" s="8"/>
@@ -876,21 +959,21 @@
     <row r="25" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="26" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
-        <v>37</v>
+        <v>31</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="3"/>
       <c r="D26" s="3" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
       <c r="E26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="3" t="s">
+        <v>9</v>
+      </c>
+      <c r="G26" s="4" t="s">
         <v>10</v>
-      </c>
-      <c r="F26" s="3" t="s">
-        <v>14</v>
-      </c>
-      <c r="G26" s="4" t="s">
-        <v>15</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
@@ -904,139 +987,155 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="5" t="s">
-        <v>8</v>
+        <v>32</v>
       </c>
       <c r="B28" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C28" s="6"/>
-      <c r="D28" s="6"/>
-      <c r="E28" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="C28" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D28" s="8"/>
+      <c r="E28" s="8"/>
       <c r="F28" s="6"/>
       <c r="G28" s="7"/>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="5" t="s">
-        <v>38</v>
+        <v>5</v>
       </c>
       <c r="B29" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C29" s="6"/>
+        <v>6</v>
+      </c>
+      <c r="C29" s="6" t="s">
+        <v>7</v>
+      </c>
       <c r="D29" s="6"/>
       <c r="E29" s="6"/>
       <c r="F29" s="6"/>
       <c r="G29" s="7"/>
     </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A30" s="5" t="s">
-        <v>39</v>
-      </c>
-      <c r="B30" s="6" t="s">
-        <v>40</v>
-      </c>
-      <c r="C30" s="6"/>
-      <c r="D30" s="6"/>
-      <c r="E30" s="6"/>
-      <c r="F30" s="6"/>
-      <c r="G30" s="7"/>
-    </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A31" s="5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B31" s="6" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="6"/>
-      <c r="D31" s="6"/>
-      <c r="E31" s="6"/>
-      <c r="F31" s="6"/>
-      <c r="G31" s="7"/>
-    </row>
-    <row r="32" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A32" s="9" t="s">
+    <row r="30" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
+        <v>35</v>
+      </c>
+      <c r="B30" s="10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C30" s="10" t="s">
+        <v>7</v>
+      </c>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="12"/>
+    </row>
+    <row r="31" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A32" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B32" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="C32" s="14"/>
+      <c r="D32" s="14"/>
+      <c r="E32" s="14"/>
+      <c r="F32" s="14"/>
+      <c r="G32" s="15"/>
+    </row>
+    <row r="33" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A33" s="5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B33" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="C33" s="6"/>
+      <c r="D33" s="6">
+        <f>66.15-5-2.5-2.99</f>
+        <v>55.660000000000004</v>
+      </c>
+      <c r="E33" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F33" s="6"/>
+      <c r="G33" s="7"/>
+    </row>
+    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A34" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="6"/>
+      <c r="D34" s="6">
+        <f>9*15</f>
+        <v>135</v>
+      </c>
+      <c r="E34" s="6" t="s">
+        <v>51</v>
+      </c>
+      <c r="F34" s="6"/>
+      <c r="G34" s="7"/>
+    </row>
+    <row r="35" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A35" s="9"/>
+      <c r="B35" s="11"/>
+      <c r="C35" s="10"/>
+      <c r="D35" s="10"/>
+      <c r="E35" s="10"/>
+      <c r="F35" s="10"/>
+      <c r="G35" s="12"/>
+    </row>
+    <row r="36" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="37" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A37" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="B37" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C37" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+      <c r="G37" s="4"/>
+    </row>
+    <row r="38" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A38" s="5" t="s">
         <v>41</v>
       </c>
-      <c r="B32" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="10"/>
-      <c r="D32" s="10"/>
-      <c r="E32" s="10"/>
-      <c r="F32" s="10"/>
-      <c r="G32" s="12"/>
-    </row>
-    <row r="33" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A34" s="2" t="s">
-        <v>20</v>
-      </c>
-      <c r="B34" s="3" t="s">
-        <v>21</v>
-      </c>
-      <c r="C34" s="14"/>
-      <c r="D34" s="14"/>
-      <c r="E34" s="14"/>
-      <c r="F34" s="14"/>
-      <c r="G34" s="15"/>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A35" s="5" t="s">
-        <v>11</v>
-      </c>
-      <c r="B35" s="6"/>
-      <c r="C35" s="6"/>
-      <c r="D35" s="6"/>
-      <c r="E35" s="6"/>
-      <c r="F35" s="6"/>
-      <c r="G35" s="7"/>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A36" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B36" s="6"/>
-      <c r="C36" s="6"/>
-      <c r="D36" s="6"/>
-      <c r="E36" s="6"/>
-      <c r="F36" s="6"/>
-      <c r="G36" s="7"/>
-    </row>
-    <row r="37" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A37" s="9" t="s">
-        <v>22</v>
-      </c>
-      <c r="B37" s="11"/>
-      <c r="C37" s="10"/>
-      <c r="D37" s="10"/>
-      <c r="E37" s="10"/>
-      <c r="F37" s="10"/>
-      <c r="G37" s="12"/>
-    </row>
-    <row r="38" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
-    <row r="39" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A39" s="2" t="s">
-        <v>17</v>
-      </c>
-      <c r="B39" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="C39" s="3" t="s">
-        <v>19</v>
-      </c>
-      <c r="D39" s="3"/>
-      <c r="E39" s="3"/>
-      <c r="F39" s="3"/>
-      <c r="G39" s="4"/>
+      <c r="B38" s="6">
+        <v>-80</v>
+      </c>
+      <c r="C38" s="6"/>
+      <c r="D38" s="6"/>
+      <c r="E38" s="6"/>
+      <c r="F38" s="6"/>
+      <c r="G38" s="7"/>
+    </row>
+    <row r="39" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A39" s="5" t="s">
+        <v>37</v>
+      </c>
+      <c r="B39" s="6"/>
+      <c r="C39" s="6">
+        <v>70</v>
+      </c>
+      <c r="D39" s="6"/>
+      <c r="E39" s="6"/>
+      <c r="F39" s="6"/>
+      <c r="G39" s="7"/>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="5" t="s">
-        <v>47</v>
-      </c>
-      <c r="B40" s="6">
-        <v>80</v>
-      </c>
+        <v>36</v>
+      </c>
+      <c r="B40" s="6"/>
       <c r="C40" s="6"/>
       <c r="D40" s="6"/>
       <c r="E40" s="6"/>
@@ -1045,10 +1144,13 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="5" t="s">
-        <v>43</v>
+        <v>7</v>
       </c>
       <c r="B41" s="6"/>
-      <c r="C41" s="6"/>
+      <c r="C41" s="6">
+        <f>10*$B$10</f>
+        <v>350</v>
+      </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
       <c r="F41" s="6"/>
@@ -1056,9 +1158,12 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="5" t="s">
-        <v>42</v>
-      </c>
-      <c r="B42" s="6"/>
+        <v>21</v>
+      </c>
+      <c r="B42" s="6">
+        <f>-(D33+D34)</f>
+        <v>-190.66</v>
+      </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
       <c r="E42" s="6"/>
@@ -1066,9 +1171,7 @@
       <c r="G42" s="7"/>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A43" s="5" t="s">
-        <v>12</v>
-      </c>
+      <c r="A43" s="5"/>
       <c r="B43" s="6"/>
       <c r="C43" s="6"/>
       <c r="D43" s="6"/>
@@ -1078,9 +1181,12 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="B44" s="6"/>
+        <v>22</v>
+      </c>
+      <c r="B44" s="6">
+        <f>-(39*2)</f>
+        <v>-78</v>
+      </c>
       <c r="C44" s="6"/>
       <c r="D44" s="6"/>
       <c r="E44" s="6"/>
@@ -1096,138 +1202,172 @@
       <c r="F45" s="6"/>
       <c r="G45" s="7"/>
     </row>
-    <row r="46" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A46" s="5" t="s">
-        <v>28</v>
-      </c>
-      <c r="B46" s="6"/>
-      <c r="C46" s="6"/>
-      <c r="D46" s="6"/>
-      <c r="E46" s="6"/>
-      <c r="F46" s="6"/>
-      <c r="G46" s="7"/>
-    </row>
-    <row r="47" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A47" s="5"/>
-      <c r="B47" s="6"/>
-      <c r="C47" s="6"/>
-      <c r="D47" s="6"/>
-      <c r="E47" s="6"/>
-      <c r="F47" s="6"/>
-      <c r="G47" s="7"/>
-    </row>
-    <row r="48" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A48" s="9" t="s">
-        <v>26</v>
-      </c>
-      <c r="B48" s="10"/>
-      <c r="C48" s="10"/>
-      <c r="D48" s="10">
-        <f>SUM(B40:B48)+SUM(C40:C48)</f>
-        <v>80</v>
-      </c>
-      <c r="E48" s="10"/>
-      <c r="F48" s="10"/>
-      <c r="G48" s="12"/>
-    </row>
-    <row r="49" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="46" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A46" s="9" t="s">
+        <v>20</v>
+      </c>
+      <c r="B46" s="10"/>
+      <c r="C46" s="10"/>
+      <c r="D46" s="10">
+        <f>SUM(B38:B46)+SUM(C38:C46)</f>
+        <v>71.340000000000032</v>
+      </c>
+      <c r="E46" s="10"/>
+      <c r="F46" s="10"/>
+      <c r="G46" s="12"/>
+    </row>
+    <row r="47" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
+    <row r="48" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A48" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="B48" s="14"/>
+      <c r="C48" s="14"/>
+      <c r="D48" s="14"/>
+      <c r="E48" s="14"/>
+      <c r="F48" s="14"/>
+      <c r="G48" s="15"/>
+    </row>
+    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A49" s="5" t="s">
+        <v>53</v>
+      </c>
+      <c r="B49" s="17">
+        <v>70</v>
+      </c>
+      <c r="C49" s="6"/>
+      <c r="D49" s="6"/>
+      <c r="E49" s="6"/>
+      <c r="F49" s="6"/>
+      <c r="G49" s="7"/>
+    </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A50" s="2" t="s">
-        <v>29</v>
-      </c>
-      <c r="B50" s="14"/>
-      <c r="C50" s="14"/>
-      <c r="D50" s="14"/>
-      <c r="E50" s="14"/>
-      <c r="F50" s="14"/>
-      <c r="G50" s="15"/>
+      <c r="A50" s="5" t="s">
+        <v>54</v>
+      </c>
+      <c r="B50" s="6">
+        <f>3*35 -D33-39</f>
+        <v>10.339999999999996</v>
+      </c>
+      <c r="C50" s="6"/>
+      <c r="D50" s="6" t="s">
+        <v>61</v>
+      </c>
+      <c r="E50" s="6"/>
+      <c r="F50" s="6"/>
+      <c r="G50" s="7"/>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A51" s="5"/>
-      <c r="B51" s="6"/>
+      <c r="A51" s="5" t="s">
+        <v>55</v>
+      </c>
+      <c r="B51" s="6">
+        <f>2*35-D34-39</f>
+        <v>-104</v>
+      </c>
       <c r="C51" s="6"/>
-      <c r="D51" s="6"/>
-      <c r="E51" s="6"/>
+      <c r="D51">
+        <f>ABS(B51)</f>
+        <v>104</v>
+      </c>
+      <c r="E51" s="6" t="s">
+        <v>62</v>
+      </c>
       <c r="F51" s="6"/>
       <c r="G51" s="7"/>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A52" s="5"/>
-      <c r="B52" s="6"/>
+      <c r="A52" s="5" t="s">
+        <v>56</v>
+      </c>
+      <c r="B52" s="6">
+        <v>35</v>
+      </c>
       <c r="C52" s="6"/>
-      <c r="D52" s="6"/>
+      <c r="D52" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
       <c r="G52" s="7"/>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A53" s="5"/>
-      <c r="B53" s="6"/>
+      <c r="A53" s="5" t="s">
+        <v>57</v>
+      </c>
+      <c r="B53" s="6">
+        <v>35</v>
+      </c>
       <c r="C53" s="6"/>
-      <c r="D53" s="6"/>
+      <c r="D53" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="7"/>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A54" s="5"/>
-      <c r="B54" s="6"/>
+      <c r="A54" s="5" t="s">
+        <v>58</v>
+      </c>
+      <c r="B54" s="8">
+        <v>35</v>
+      </c>
       <c r="C54" s="6"/>
-      <c r="D54" s="6"/>
+      <c r="D54" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
       <c r="G54" s="7"/>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A55" s="5"/>
-      <c r="B55" s="6"/>
+      <c r="A55" s="16" t="s">
+        <v>59</v>
+      </c>
+      <c r="B55" s="8">
+        <v>35</v>
+      </c>
       <c r="C55" s="6"/>
-      <c r="D55" s="6"/>
+      <c r="D55" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="7"/>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A56" s="5"/>
-      <c r="B56" s="6"/>
+      <c r="A56" s="5" t="s">
+        <v>60</v>
+      </c>
+      <c r="B56" s="8">
+        <v>35</v>
+      </c>
       <c r="C56" s="6"/>
-      <c r="D56" s="6"/>
+      <c r="D56" s="6" t="s">
+        <v>61</v>
+      </c>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A57" s="16"/>
-      <c r="B57" s="6"/>
-      <c r="C57" s="6"/>
-      <c r="D57" s="6"/>
-      <c r="E57" s="6"/>
-      <c r="F57" s="6"/>
-      <c r="G57" s="7"/>
-    </row>
-    <row r="58" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A58" s="5"/>
-      <c r="B58" s="6"/>
-      <c r="C58" s="6"/>
-      <c r="D58" s="6"/>
-      <c r="E58" s="6"/>
-      <c r="F58" s="6"/>
-      <c r="G58" s="7"/>
-    </row>
-    <row r="59" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A59" s="9"/>
-      <c r="B59" s="10"/>
-      <c r="C59" s="10"/>
-      <c r="D59" s="10"/>
-      <c r="E59" s="10"/>
-      <c r="F59" s="10"/>
-      <c r="G59" s="12"/>
+    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="9"/>
+      <c r="B57" s="10"/>
+      <c r="C57" s="10"/>
+      <c r="D57" s="10"/>
+      <c r="E57" s="18">
+        <f>SUM(B49:B56)+B38-D46</f>
+        <v>0</v>
+      </c>
+      <c r="F57" s="10"/>
+      <c r="G57" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A6:G6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup scale="88" orientation="portrait" r:id="rId1"/>
+  <pageSetup scale="79" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Updated Joshua Tree accounting
</commit_message>
<xml_diff>
--- a/events/Joshua_Tree_2019/JoshuaTree2019.xlsx
+++ b/events/Joshua_Tree_2019/JoshuaTree2019.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="63">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
   <si>
     <t>Patrol</t>
   </si>
@@ -163,9 +163,6 @@
     <t>Stephan</t>
   </si>
   <si>
-    <t>Schuster</t>
-  </si>
-  <si>
     <t>chk</t>
   </si>
   <si>
@@ -205,15 +202,31 @@
     <t>debit</t>
   </si>
   <si>
-    <t>credit to Schuster account</t>
+    <t>Pauly</t>
+  </si>
+  <si>
+    <t>Pauly SA</t>
+  </si>
+  <si>
+    <t>credit to Pauly account</t>
+  </si>
+  <si>
+    <t>credit to Stephan account</t>
+  </si>
+  <si>
+    <t>(changed from $35)</t>
+  </si>
+  <si>
+    <t>actual total</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
+    <numFmt numFmtId="8" formatCode="&quot;$&quot;#,##0.00_);[Red]\(&quot;$&quot;#,##0.00\)"/>
   </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
@@ -332,7 +345,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="21">
+  <cellXfs count="23">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -352,6 +365,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="6" fontId="0" fillId="0" borderId="7" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="8" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -665,10 +680,10 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:G57"/>
+  <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:G57"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="A59" sqref="A59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -736,15 +751,15 @@
       <c r="G5" s="7"/>
     </row>
     <row r="6" spans="1:7" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="19" t="s">
+      <c r="A6" s="21" t="s">
         <v>40</v>
       </c>
-      <c r="B6" s="19"/>
-      <c r="C6" s="19"/>
-      <c r="D6" s="19"/>
-      <c r="E6" s="19"/>
-      <c r="F6" s="19"/>
-      <c r="G6" s="20"/>
+      <c r="B6" s="21"/>
+      <c r="C6" s="21"/>
+      <c r="D6" s="21"/>
+      <c r="E6" s="21"/>
+      <c r="F6" s="21"/>
+      <c r="G6" s="22"/>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="5"/>
@@ -766,10 +781,13 @@
     </row>
     <row r="10" spans="1:7" s="1" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B10" s="1">
-        <v>35</v>
+        <v>30</v>
+      </c>
+      <c r="D10" s="1" t="s">
+        <v>65</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -859,7 +877,7 @@
         <v>7</v>
       </c>
       <c r="D17" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E17" s="6"/>
       <c r="F17" s="6"/>
@@ -871,10 +889,10 @@
       </c>
       <c r="B18" s="6"/>
       <c r="C18" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D18" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="D18" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="E18" s="6"/>
       <c r="F18" s="6"/>
@@ -886,10 +904,10 @@
       </c>
       <c r="B19" s="6"/>
       <c r="C19" s="8" t="s">
+        <v>48</v>
+      </c>
+      <c r="D19" s="8" t="s">
         <v>49</v>
-      </c>
-      <c r="D19" s="8" t="s">
-        <v>50</v>
       </c>
       <c r="E19" s="6"/>
       <c r="F19" s="8"/>
@@ -904,7 +922,7 @@
         <v>7</v>
       </c>
       <c r="D20" s="8" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E20" s="6"/>
       <c r="F20" s="8"/>
@@ -1053,11 +1071,11 @@
       </c>
       <c r="C33" s="6"/>
       <c r="D33" s="6">
-        <f>66.15-5-2.5-2.99</f>
-        <v>55.660000000000004</v>
+        <f>66.15+6.45-5-2.5-2.99</f>
+        <v>62.110000000000007</v>
       </c>
       <c r="E33" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F33" s="6"/>
       <c r="G33" s="7"/>
@@ -1067,15 +1085,14 @@
         <v>46</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>48</v>
+        <v>61</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6">
-        <f>9*15</f>
-        <v>135</v>
+        <v>116.35</v>
       </c>
       <c r="E34" s="6" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="F34" s="6"/>
       <c r="G34" s="7"/>
@@ -1149,7 +1166,7 @@
       <c r="B41" s="6"/>
       <c r="C41" s="6">
         <f>10*$B$10</f>
-        <v>350</v>
+        <v>300</v>
       </c>
       <c r="D41" s="6"/>
       <c r="E41" s="6"/>
@@ -1162,7 +1179,7 @@
       </c>
       <c r="B42" s="6">
         <f>-(D33+D34)</f>
-        <v>-190.66</v>
+        <v>-178.46</v>
       </c>
       <c r="C42" s="6"/>
       <c r="D42" s="6"/>
@@ -1210,7 +1227,7 @@
       <c r="C46" s="10"/>
       <c r="D46" s="10">
         <f>SUM(B38:B46)+SUM(C38:C46)</f>
-        <v>71.340000000000032</v>
+        <v>33.539999999999964</v>
       </c>
       <c r="E46" s="10"/>
       <c r="F46" s="10"/>
@@ -1228,9 +1245,9 @@
       <c r="F48" s="14"/>
       <c r="G48" s="15"/>
     </row>
-    <row r="49" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B49" s="17">
         <v>70</v>
@@ -1241,127 +1258,149 @@
       <c r="F49" s="6"/>
       <c r="G49" s="7"/>
     </row>
-    <row r="50" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="5" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B50" s="6">
-        <f>3*35 -D33-39</f>
-        <v>10.339999999999996</v>
+        <f>3*$B$10-D33-39</f>
+        <v>-11.110000000000007</v>
       </c>
       <c r="C50" s="6"/>
-      <c r="D50" s="6" t="s">
-        <v>61</v>
-      </c>
-      <c r="E50" s="6"/>
+      <c r="D50" s="6">
+        <f>ABS(B50)</f>
+        <v>11.110000000000007</v>
+      </c>
+      <c r="E50" s="6" t="s">
+        <v>64</v>
+      </c>
       <c r="F50" s="6"/>
       <c r="G50" s="7"/>
     </row>
-    <row r="51" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="5" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B51" s="6">
-        <f>2*35-D34-39</f>
-        <v>-104</v>
+        <f>2*$B$10-39</f>
+        <v>21</v>
       </c>
       <c r="C51" s="6"/>
-      <c r="D51">
-        <f>ABS(B51)</f>
-        <v>104</v>
-      </c>
-      <c r="E51" s="6" t="s">
-        <v>62</v>
-      </c>
+      <c r="D51" t="s">
+        <v>60</v>
+      </c>
+      <c r="E51" s="6"/>
       <c r="F51" s="6"/>
       <c r="G51" s="7"/>
     </row>
-    <row r="52" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="5" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B52" s="6">
-        <v>35</v>
+        <f>$B$10</f>
+        <v>30</v>
       </c>
       <c r="C52" s="6"/>
       <c r="D52" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E52" s="6"/>
       <c r="F52" s="6"/>
       <c r="G52" s="7"/>
-    </row>
-    <row r="53" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I52" s="20"/>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="5" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B53" s="6">
-        <v>35</v>
+        <f>$B$10</f>
+        <v>30</v>
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
       <c r="G53" s="7"/>
     </row>
-    <row r="54" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="5" t="s">
-        <v>58</v>
-      </c>
-      <c r="B54" s="8">
-        <v>35</v>
+        <v>57</v>
+      </c>
+      <c r="B54" s="6">
+        <f>$B$10</f>
+        <v>30</v>
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
-      <c r="G54" s="7"/>
-    </row>
-    <row r="55" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="19"/>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55" s="16" t="s">
-        <v>59</v>
-      </c>
-      <c r="B55" s="8">
-        <v>35</v>
+        <v>58</v>
+      </c>
+      <c r="B55" s="6">
+        <f>$B$10</f>
+        <v>30</v>
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
       <c r="G55" s="7"/>
     </row>
-    <row r="56" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>60</v>
-      </c>
-      <c r="B56" s="8">
-        <v>35</v>
+        <v>59</v>
+      </c>
+      <c r="B56" s="6">
+        <f>$B$10</f>
+        <v>30</v>
       </c>
       <c r="C56" s="6"/>
       <c r="D56" s="6" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
       <c r="G56" s="7"/>
     </row>
-    <row r="57" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A57" s="9"/>
-      <c r="B57" s="10"/>
+    <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A57" s="9" t="s">
+        <v>62</v>
+      </c>
+      <c r="B57" s="10">
+        <f>-D34-2*5</f>
+        <v>-126.35</v>
+      </c>
       <c r="C57" s="10"/>
-      <c r="D57" s="10"/>
-      <c r="E57" s="18">
-        <f>SUM(B49:B56)+B38-D46</f>
-        <v>0</v>
+      <c r="D57" s="10">
+        <f>ABS(B57)</f>
+        <v>126.35</v>
+      </c>
+      <c r="E57" s="18" t="s">
+        <v>63</v>
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="12"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="D59" t="s">
+        <v>66</v>
+      </c>
+      <c r="E59" s="20">
+        <f>SUM(B49:B57)+B38</f>
+        <v>23.539999999999992</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>

<commit_message>
Cleaning up PII directory
</commit_message>
<xml_diff>
--- a/events/Joshua_Tree_2019/JoshuaTree2019.xlsx
+++ b/events/Joshua_Tree_2019/JoshuaTree2019.xlsx
@@ -17,7 +17,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="67">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="67">
   <si>
     <t>Patrol</t>
   </si>
@@ -196,9 +196,6 @@
     <t>Dion Roer SA</t>
   </si>
   <si>
-    <t>Arita SA</t>
-  </si>
-  <si>
     <t>debit</t>
   </si>
   <si>
@@ -218,6 +215,9 @@
   </si>
   <si>
     <t>actual total</t>
+  </si>
+  <si>
+    <t>credit to Maclean account</t>
   </si>
 </sst>
 </file>
@@ -682,8 +682,8 @@
   </sheetPr>
   <dimension ref="A1:I59"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
-      <selection activeCell="A59" sqref="A59"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A54" sqref="A54"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -787,7 +787,7 @@
         <v>30</v>
       </c>
       <c r="D10" s="1" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
@@ -844,7 +844,7 @@
         <v>28</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D15" s="6" t="s">
         <v>28</v>
@@ -934,7 +934,7 @@
       </c>
       <c r="B21" s="6"/>
       <c r="C21" s="8" t="s">
-        <v>7</v>
+        <v>48</v>
       </c>
       <c r="D21" s="6"/>
       <c r="E21" s="6"/>
@@ -1085,7 +1085,7 @@
         <v>46</v>
       </c>
       <c r="B34" s="8" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C34" s="6"/>
       <c r="D34" s="6">
@@ -1250,7 +1250,7 @@
         <v>52</v>
       </c>
       <c r="B49" s="17">
-        <v>70</v>
+        <v>135</v>
       </c>
       <c r="C49" s="6"/>
       <c r="D49" s="6"/>
@@ -1272,7 +1272,7 @@
         <v>11.110000000000007</v>
       </c>
       <c r="E50" s="6" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="F50" s="6"/>
       <c r="G50" s="7"/>
@@ -1287,7 +1287,7 @@
       </c>
       <c r="C51" s="6"/>
       <c r="D51" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E51" s="6"/>
       <c r="F51" s="6"/>
@@ -1298,14 +1298,16 @@
         <v>55</v>
       </c>
       <c r="B52" s="6">
-        <f>$B$10</f>
-        <v>30</v>
+        <v>-5</v>
       </c>
       <c r="C52" s="6"/>
-      <c r="D52" s="6" t="s">
-        <v>60</v>
-      </c>
-      <c r="E52" s="6"/>
+      <c r="D52" s="6">
+        <f>ABS(B52)</f>
+        <v>5</v>
+      </c>
+      <c r="E52" s="6" t="s">
+        <v>66</v>
+      </c>
       <c r="F52" s="6"/>
       <c r="G52" s="7"/>
       <c r="I52" s="20"/>
@@ -1320,7 +1322,7 @@
       </c>
       <c r="C53" s="6"/>
       <c r="D53" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E53" s="6"/>
       <c r="F53" s="6"/>
@@ -1336,7 +1338,7 @@
       </c>
       <c r="C54" s="6"/>
       <c r="D54" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E54" s="6"/>
       <c r="F54" s="6"/>
@@ -1352,7 +1354,7 @@
       </c>
       <c r="C55" s="6"/>
       <c r="D55" s="6" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="E55" s="6"/>
       <c r="F55" s="6"/>
@@ -1360,15 +1362,16 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="5" t="s">
-        <v>59</v>
-      </c>
-      <c r="B56" s="6">
-        <f>$B$10</f>
-        <v>30</v>
-      </c>
-      <c r="C56" s="6"/>
+        <v>28</v>
+      </c>
+      <c r="B56" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C56" s="6" t="s">
+        <v>28</v>
+      </c>
       <c r="D56" s="6" t="s">
-        <v>60</v>
+        <v>28</v>
       </c>
       <c r="E56" s="6"/>
       <c r="F56" s="6"/>
@@ -1376,7 +1379,7 @@
     </row>
     <row r="57" spans="1:9" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A57" s="9" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B57" s="10">
         <f>-D34-2*5</f>
@@ -1388,14 +1391,14 @@
         <v>126.35</v>
       </c>
       <c r="E57" s="18" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="F57" s="10"/>
       <c r="G57" s="12"/>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="D59" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E59" s="20">
         <f>SUM(B49:B57)+B38</f>

</xml_diff>